<commit_message>
prepared for all products
</commit_message>
<xml_diff>
--- a/data/bgm_combined_results_df_250203_part1.xlsx
+++ b/data/bgm_combined_results_df_250203_part1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiyuantao/Desktop/Mac科研/experiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15820983-0FAD-654A-A0F6-5EAED505CF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0F5C85-B2B3-4F46-BD6F-728217793635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8260" yWindow="1020" windowWidth="30240" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bgm_combined_results_df_250203_" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="1655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="1656">
   <si>
     <t>sid</t>
   </si>
@@ -4993,6 +4993,10 @@
   </si>
   <si>
     <t>[30]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -5000,7 +5004,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5034,6 +5038,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5056,7 +5067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5068,6 +5079,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5288,13 +5302,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="J239" sqref="J239"/>
+    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="C247" sqref="C247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12870,23 +12886,80 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="240" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="3">
+        <v>20001</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>1655</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="J240" s="4" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="3">
+        <v>30001</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>1655</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="G241" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="J241" s="4" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="3">
+        <v>40001</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>1655</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="G242" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="J242" s="4" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="257" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="258" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="259" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13640,6 +13713,9 @@
     <hyperlink ref="J237" r:id="rId4" xr:uid="{0124D88D-6C9B-0F47-B7E1-E105C22C824E}"/>
     <hyperlink ref="J235" r:id="rId5" xr:uid="{2C4876DE-4DA4-5B40-AE55-CCE3E2898DFC}"/>
     <hyperlink ref="J236" r:id="rId6" xr:uid="{499D9B14-2B68-384B-888F-A8BA5AA467E1}"/>
+    <hyperlink ref="J240" r:id="rId7" xr:uid="{E5275627-327E-DB4B-9405-637062D0836F}"/>
+    <hyperlink ref="J241" r:id="rId8" xr:uid="{11300CA1-5B8C-B541-95C9-54A7662DC38B}"/>
+    <hyperlink ref="J242" r:id="rId9" xr:uid="{587130D8-6BD5-5242-B227-9FAA318DF5BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>